<commit_message>
diminuindo linhas de codigo
</commit_message>
<xml_diff>
--- a/produtos_consoles.xlsx
+++ b/produtos_consoles.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25409"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB9C0390-C68C-4FDE-8A17-E00A2189BEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA83AFA5-8757-4C7D-883E-5F6F59C341FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="consultas" sheetId="1" r:id="rId1"/>
+    <sheet name="consoles" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="46">
   <si>
     <t>PRODUTOS</t>
   </si>
@@ -50,30 +52,105 @@
     <t>EMAIL</t>
   </si>
   <si>
+    <t>CONSOLE ATARI</t>
+  </si>
+  <si>
+    <t>ATARI</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>ghost importados</t>
+  </si>
+  <si>
+    <t>11943436565</t>
+  </si>
+  <si>
+    <t>ghost@importados.com.br</t>
+  </si>
+  <si>
+    <t>CONSOLE PHANTOM SYSTEM</t>
+  </si>
+  <si>
+    <t>GRADIENTE</t>
+  </si>
+  <si>
+    <t>CONSOLE XBOX</t>
+  </si>
+  <si>
+    <t>MICROSOFT</t>
+  </si>
+  <si>
+    <t>SHOGUN IMPORTS</t>
+  </si>
+  <si>
+    <t>11986865454</t>
+  </si>
+  <si>
+    <t>shogun@imports.com</t>
+  </si>
+  <si>
+    <t>CONSOLE XBOX 360</t>
+  </si>
+  <si>
+    <t>CONSOLE XBOX 360 Slim</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Shogun Imports</t>
+  </si>
+  <si>
+    <t>CONSOLE XBOX ONE</t>
+  </si>
+  <si>
+    <t>CONSOLE XBOX Series X/S</t>
+  </si>
+  <si>
+    <t>CONSOLE SUPER NINTENDO</t>
+  </si>
+  <si>
+    <t>NINTENDO</t>
+  </si>
+  <si>
+    <t>Ghost Importados</t>
+  </si>
+  <si>
+    <t>CONSOLE NINTENDO 64</t>
+  </si>
+  <si>
+    <t>CONSOLE NINTENDO WII</t>
+  </si>
+  <si>
+    <t>CONSOLE NINTENDO WII U</t>
+  </si>
+  <si>
+    <t>CONSOLE NINTENDO SWITCH</t>
+  </si>
+  <si>
+    <t>CONSOLE MEGA DRIVE</t>
+  </si>
+  <si>
+    <t>SEGA</t>
+  </si>
+  <si>
+    <t>CONSOLE SATURN</t>
+  </si>
+  <si>
+    <t>CONSOLE DREAMCAST</t>
+  </si>
+  <si>
     <t>CONSOLE PLAYSTATION 1</t>
   </si>
   <si>
     <t>SONY</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Shogun Imports</t>
-  </si>
-  <si>
-    <t>11986865454</t>
-  </si>
-  <si>
-    <t>shogun@imports.com</t>
-  </si>
-  <si>
     <t>CONSOLE PLAYSTATION 2</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>CONSOLE PLAYSTATION 2 Slim</t>
   </si>
   <si>
@@ -90,82 +167,13 @@
   </si>
   <si>
     <t>CONSOLE PLAYSTATION 4 Pro</t>
-  </si>
-  <si>
-    <t>CONSOLE XBOX</t>
-  </si>
-  <si>
-    <t>MICROSOFT</t>
-  </si>
-  <si>
-    <t>CONSOLE XBOX 360</t>
-  </si>
-  <si>
-    <t>CONSOLE XBOX 360 Slim</t>
-  </si>
-  <si>
-    <t>CONSOLE XBOX ONE</t>
-  </si>
-  <si>
-    <t>CONSOLE XBOX Series X/S</t>
-  </si>
-  <si>
-    <t>CONSOLE SUPER NINTENDO</t>
-  </si>
-  <si>
-    <t>NINTENDO</t>
-  </si>
-  <si>
-    <t>Ghost Importados LTDA</t>
-  </si>
-  <si>
-    <t>11943436565</t>
-  </si>
-  <si>
-    <t>ghost@importados.com.br</t>
-  </si>
-  <si>
-    <t>CONSOLE SEGA MEGA DRIVE</t>
-  </si>
-  <si>
-    <t>SEGA</t>
-  </si>
-  <si>
-    <t>CONSOLE SEGA SATURNO</t>
-  </si>
-  <si>
-    <t>CONSOLE SEGA DREAMCAST</t>
-  </si>
-  <si>
-    <t>CONSOLE NINTENDO 64</t>
-  </si>
-  <si>
-    <t>CONSOLE ATARI</t>
-  </si>
-  <si>
-    <t>ATARI</t>
-  </si>
-  <si>
-    <t>CONSOLE PHANTOM SYSTEM</t>
-  </si>
-  <si>
-    <t>GRADIENTE</t>
-  </si>
-  <si>
-    <t>CONSOLE NINTENDO WII</t>
-  </si>
-  <si>
-    <t>CONSOLE NINTENDO WII U</t>
-  </si>
-  <si>
-    <t>CONSOLE NINTENDO SWITCH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -185,13 +193,26 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAEAAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -214,13 +235,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -443,12 +465,12 @@
   <dimension ref="A1:G955"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="36.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="2"/>
     <col min="4" max="4" width="12.5703125" style="1"/>
@@ -459,25 +481,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -489,7 +511,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2">
-        <v>500</v>
+        <v>470</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -509,13 +531,13 @@
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>10</v>
@@ -532,131 +554,131 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2">
-        <v>900</v>
+        <v>450</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12.75">
       <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" s="2">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2">
-        <v>1500</v>
+        <v>1250</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75">
       <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1700</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2000</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="G7" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75">
       <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4500</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2300</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2">
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>11</v>
@@ -667,19 +689,19 @@
     </row>
     <row r="10" spans="1:7" ht="12.75">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>11</v>
@@ -690,19 +712,19 @@
     </row>
     <row r="11" spans="1:7" ht="12.75">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2">
-        <v>1100</v>
+        <v>600</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>11</v>
@@ -713,19 +735,19 @@
     </row>
     <row r="12" spans="1:7" ht="12.75">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2">
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>11</v>
@@ -736,19 +758,19 @@
     </row>
     <row r="13" spans="1:7" ht="12.75">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="2">
-        <v>1700</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
@@ -759,19 +781,19 @@
     </row>
     <row r="14" spans="1:7" ht="12.75">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2">
+        <v>550</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="2">
-        <v>4500</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>11</v>
@@ -782,232 +804,232 @@
     </row>
     <row r="15" spans="1:7" ht="12.75">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="12.75">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2">
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.75">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2">
-        <v>450</v>
+        <v>800</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2">
-        <v>400</v>
+        <v>900</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="2">
-        <v>470</v>
+        <v>1300</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2">
-        <v>1500</v>
+        <v>2300</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:7"/>
@@ -1942,12 +1964,39 @@
     <row r="954"/>
     <row r="955"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G24">
+    <sortCondition ref="B2:B24"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{63A4E8AE-52B6-4DD1-839B-5A04EACC8EA6}"/>
-    <hyperlink ref="G15" r:id="rId2" xr:uid="{4D927242-FC9D-4551-AC9A-33FC258BC997}"/>
+    <hyperlink ref="G17" r:id="rId1" xr:uid="{63A4E8AE-52B6-4DD1-839B-5A04EACC8EA6}"/>
+    <hyperlink ref="G9" r:id="rId2" xr:uid="{4D927242-FC9D-4551-AC9A-33FC258BC997}"/>
     <hyperlink ref="G3:G14" r:id="rId3" display="shogun@imports.com" xr:uid="{725213E1-DCF2-4E81-B26E-73B1D7C7C472}"/>
     <hyperlink ref="G16:G24" r:id="rId4" display="ghost@importados.com.br" xr:uid="{2E3EC517-61CC-439A-9F65-040171E19DCC}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E875187-0E2A-4390-A04B-E24390E91FB0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05C3B5-B387-4663-A738-B743EEC71D58}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>